<commit_message>
adding trajectory using district = Kanpur city
</commit_message>
<xml_diff>
--- a/Results/trajectory.xlsx
+++ b/Results/trajectory.xlsx
@@ -418,10 +418,10 @@
         <v>43478</v>
       </c>
       <c r="D2">
-        <v>25.02951183303265</v>
+        <v>25.97914421306509</v>
       </c>
       <c r="E2">
-        <v>80.69673029266555</v>
+        <v>80.54366902288416</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -435,10 +435,10 @@
         <v>43478.04166666666</v>
       </c>
       <c r="D3">
-        <v>24.80987615681973</v>
+        <v>25.98941348494238</v>
       </c>
       <c r="E3">
-        <v>80.6339029205988</v>
+        <v>80.68467629199473</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -452,10 +452,10 @@
         <v>43478.08333333334</v>
       </c>
       <c r="D4">
-        <v>24.73079380288324</v>
+        <v>26.05187325770935</v>
       </c>
       <c r="E4">
-        <v>80.3768482363436</v>
+        <v>80.53762068302292</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -469,10 +469,10 @@
         <v>43478.125</v>
       </c>
       <c r="D5">
-        <v>24.90427656412486</v>
+        <v>26.09224605891093</v>
       </c>
       <c r="E5">
-        <v>80.28220825144405</v>
+        <v>80.64300504726322</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -486,10 +486,10 @@
         <v>43478.16666666666</v>
       </c>
       <c r="D6">
-        <v>24.43895336398839</v>
+        <v>25.99723548246855</v>
       </c>
       <c r="E6">
-        <v>80.30387584108283</v>
+        <v>80.6814421474746</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -503,10 +503,10 @@
         <v>43478.20833333334</v>
       </c>
       <c r="D7">
-        <v>24.53291947085037</v>
+        <v>26.12007639273669</v>
       </c>
       <c r="E7">
-        <v>79.97908553560359</v>
+        <v>80.65914760059353</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -520,10 +520,10 @@
         <v>43478.25</v>
       </c>
       <c r="D8">
-        <v>24.48506023260159</v>
+        <v>26.10887519321162</v>
       </c>
       <c r="E8">
-        <v>80.24308223982835</v>
+        <v>80.66388680155235</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -537,10 +537,10 @@
         <v>43478.29166666666</v>
       </c>
       <c r="D9">
-        <v>24.36497131068206</v>
+        <v>26.01597925778497</v>
       </c>
       <c r="E9">
-        <v>80.13519682862757</v>
+        <v>80.61595055530151</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -554,10 +554,10 @@
         <v>43478.33333333334</v>
       </c>
       <c r="D10">
-        <v>24.34355277053268</v>
+        <v>26.010313764674</v>
       </c>
       <c r="E10">
-        <v>80.34854721640825</v>
+        <v>80.67132435363075</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -571,10 +571,10 @@
         <v>43478.375</v>
       </c>
       <c r="D11">
-        <v>24.47777665655232</v>
+        <v>26.00480147063099</v>
       </c>
       <c r="E11">
-        <v>80.0695873515412</v>
+        <v>80.6485501039148</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -588,10 +588,10 @@
         <v>43478.41666666666</v>
       </c>
       <c r="D12">
-        <v>24.5801778582184</v>
+        <v>25.97124369110383</v>
       </c>
       <c r="E12">
-        <v>80.17382091395949</v>
+        <v>80.64230412452288</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -605,10 +605,10 @@
         <v>43478.45833333334</v>
       </c>
       <c r="D13">
-        <v>24.51921537880596</v>
+        <v>26.07169211249931</v>
       </c>
       <c r="E13">
-        <v>79.99214963635823</v>
+        <v>80.65462530947816</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -622,10 +622,10 @@
         <v>43478.5</v>
       </c>
       <c r="D14">
-        <v>24.50914174459596</v>
+        <v>26.08596289211871</v>
       </c>
       <c r="E14">
-        <v>80.32466579470668</v>
+        <v>80.68689141197429</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -639,10 +639,10 @@
         <v>43478.54166666666</v>
       </c>
       <c r="D15">
-        <v>24.67153810232205</v>
+        <v>26.06404775583821</v>
       </c>
       <c r="E15">
-        <v>80.03356176439482</v>
+        <v>80.53585967459412</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -656,10 +656,10 @@
         <v>43478.58333333334</v>
       </c>
       <c r="D16">
-        <v>24.69757053968209</v>
+        <v>26.13808184191592</v>
       </c>
       <c r="E16">
-        <v>79.97490907536829</v>
+        <v>80.447539251382</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -673,10 +673,10 @@
         <v>43478.625</v>
       </c>
       <c r="D17">
-        <v>25.2208268203206</v>
+        <v>26.01010184946066</v>
       </c>
       <c r="E17">
-        <v>80.10878969788361</v>
+        <v>80.29110045011549</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -690,10 +690,10 @@
         <v>43478.66666666666</v>
       </c>
       <c r="D18">
-        <v>25.07380105218638</v>
+        <v>25.96634721504069</v>
       </c>
       <c r="E18">
-        <v>80.31657443073624</v>
+        <v>80.36249612454891</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -707,10 +707,10 @@
         <v>43478.70833333334</v>
       </c>
       <c r="D19">
-        <v>25.2392962508873</v>
+        <v>26.03577928324084</v>
       </c>
       <c r="E19">
-        <v>80.06433031619663</v>
+        <v>80.36475235317971</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -724,10 +724,10 @@
         <v>43478.75</v>
       </c>
       <c r="D20">
-        <v>25.05783731324794</v>
+        <v>26.10858100736315</v>
       </c>
       <c r="E20">
-        <v>79.89971551969285</v>
+        <v>80.29574834325317</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -741,10 +741,10 @@
         <v>43478.79166666666</v>
       </c>
       <c r="D21">
-        <v>25.34605083040939</v>
+        <v>26.1491975147379</v>
       </c>
       <c r="E21">
-        <v>79.77886447046293</v>
+        <v>80.36993447794623</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -758,10 +758,10 @@
         <v>43478.83333333334</v>
       </c>
       <c r="D22">
-        <v>25.1077339011319</v>
+        <v>26.08736218296248</v>
       </c>
       <c r="E22">
-        <v>79.73592742436298</v>
+        <v>80.35075691096442</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -775,10 +775,10 @@
         <v>43478.875</v>
       </c>
       <c r="D23">
-        <v>25.25822045045034</v>
+        <v>26.09290942205135</v>
       </c>
       <c r="E23">
-        <v>80.06124247978951</v>
+        <v>80.31997337317584</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -792,10 +792,10 @@
         <v>43478.91666666666</v>
       </c>
       <c r="D24">
-        <v>25.03978568152385</v>
+        <v>25.97214064921764</v>
       </c>
       <c r="E24">
-        <v>80.24864819226148</v>
+        <v>80.31811162705594</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -809,10 +809,10 @@
         <v>43478.95833333334</v>
       </c>
       <c r="D25">
-        <v>25.31581185992859</v>
+        <v>26.04129379978499</v>
       </c>
       <c r="E25">
-        <v>80.1089246664894</v>
+        <v>80.38066626112563</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -826,10 +826,10 @@
         <v>43478</v>
       </c>
       <c r="D26">
-        <v>24.95513073180832</v>
+        <v>26.62766608408358</v>
       </c>
       <c r="E26">
-        <v>79.07752364046063</v>
+        <v>80.24292172850279</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -843,10 +843,10 @@
         <v>43478.04166666666</v>
       </c>
       <c r="D27">
-        <v>24.73474518550042</v>
+        <v>26.48427071500427</v>
       </c>
       <c r="E27">
-        <v>79.09417848287517</v>
+        <v>80.22061842339515</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -860,10 +860,10 @@
         <v>43478.08333333334</v>
       </c>
       <c r="D28">
-        <v>24.98392651052298</v>
+        <v>26.74171008405407</v>
       </c>
       <c r="E28">
-        <v>79.1536223966627</v>
+        <v>80.19832302607881</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -877,10 +877,10 @@
         <v>43478.125</v>
       </c>
       <c r="D29">
-        <v>24.85713157391976</v>
+        <v>26.48874428580262</v>
       </c>
       <c r="E29">
-        <v>79.2737518048655</v>
+        <v>80.25416676985792</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -894,10 +894,10 @@
         <v>43478.16666666666</v>
       </c>
       <c r="D30">
-        <v>24.99444567140228</v>
+        <v>26.60606501686484</v>
       </c>
       <c r="E30">
-        <v>79.19486481009795</v>
+        <v>80.25067102111996</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -911,10 +911,10 @@
         <v>43478.20833333334</v>
       </c>
       <c r="D31">
-        <v>24.40977763369195</v>
+        <v>26.44440552147264</v>
       </c>
       <c r="E31">
-        <v>79.22785873272909</v>
+        <v>80.26945890918813</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -928,10 +928,10 @@
         <v>43478.25</v>
       </c>
       <c r="D32">
-        <v>25.02151617842764</v>
+        <v>26.55469009925863</v>
       </c>
       <c r="E32">
-        <v>79.13032974973193</v>
+        <v>80.25158336426746</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -945,10 +945,10 @@
         <v>43478.29166666666</v>
       </c>
       <c r="D33">
-        <v>24.85868671696441</v>
+        <v>26.45451853990314</v>
       </c>
       <c r="E33">
-        <v>79.27411642985307</v>
+        <v>80.19623545446885</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -962,10 +962,10 @@
         <v>43478.33333333334</v>
       </c>
       <c r="D34">
-        <v>24.40225326979555</v>
+        <v>26.66330376023499</v>
       </c>
       <c r="E34">
-        <v>79.17460961759856</v>
+        <v>80.1940624239874</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -979,10 +979,10 @@
         <v>43478.375</v>
       </c>
       <c r="D35">
-        <v>24.97916629812472</v>
+        <v>26.38039367469273</v>
       </c>
       <c r="E35">
-        <v>79.23255491553574</v>
+        <v>80.21394353518977</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -996,10 +996,10 @@
         <v>43478.41666666666</v>
       </c>
       <c r="D36">
-        <v>24.73012589904308</v>
+        <v>26.70380761333309</v>
       </c>
       <c r="E36">
-        <v>79.13153229122786</v>
+        <v>80.25124981774981</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1013,10 +1013,10 @@
         <v>43478.45833333334</v>
       </c>
       <c r="D37">
-        <v>24.67661943442723</v>
+        <v>26.43311481876193</v>
       </c>
       <c r="E37">
-        <v>79.1184023411697</v>
+        <v>80.26619639474406</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1030,10 +1030,10 @@
         <v>43478.5</v>
       </c>
       <c r="D38">
-        <v>24.96584927102138</v>
+        <v>26.67314554057378</v>
       </c>
       <c r="E38">
-        <v>79.13856779965774</v>
+        <v>80.24673309269829</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1047,10 +1047,10 @@
         <v>43478.54166666666</v>
       </c>
       <c r="D39">
-        <v>24.92429219498441</v>
+        <v>26.38200487822357</v>
       </c>
       <c r="E39">
-        <v>79.28276846336574</v>
+        <v>80.20538538230437</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1064,10 +1064,10 @@
         <v>43478.58333333334</v>
       </c>
       <c r="D40">
-        <v>24.76681206632586</v>
+        <v>26.60543167134669</v>
       </c>
       <c r="E40">
-        <v>79.21597315653811</v>
+        <v>80.24464410841229</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1081,10 +1081,10 @@
         <v>43478.625</v>
       </c>
       <c r="D41">
-        <v>24.9450332814332</v>
+        <v>26.36167812741875</v>
       </c>
       <c r="E41">
-        <v>79.23474441013158</v>
+        <v>80.25247216590274</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1098,10 +1098,10 @@
         <v>43478.66666666666</v>
       </c>
       <c r="D42">
-        <v>24.67547379625466</v>
+        <v>26.43668384961671</v>
       </c>
       <c r="E42">
-        <v>79.27311198160344</v>
+        <v>80.37073705024702</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1115,10 +1115,10 @@
         <v>43478.70833333334</v>
       </c>
       <c r="D43">
-        <v>25.02450253115337</v>
+        <v>26.53739566943603</v>
       </c>
       <c r="E43">
-        <v>79.2771816845202</v>
+        <v>80.47392935626137</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1132,10 +1132,10 @@
         <v>43478.75</v>
       </c>
       <c r="D44">
-        <v>24.69284883551515</v>
+        <v>26.5123958966421</v>
       </c>
       <c r="E44">
-        <v>79.17443360484597</v>
+        <v>80.32047782654158</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1149,10 +1149,10 @@
         <v>43478.79166666666</v>
       </c>
       <c r="D45">
-        <v>24.96302428353203</v>
+        <v>26.40845183631535</v>
       </c>
       <c r="E45">
-        <v>79.20441538715922</v>
+        <v>80.43052942182881</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1166,10 +1166,10 @@
         <v>43478.83333333334</v>
       </c>
       <c r="D46">
-        <v>25.01210357613916</v>
+        <v>26.3813515431657</v>
       </c>
       <c r="E46">
-        <v>79.07495246391358</v>
+        <v>80.28346923611215</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1183,10 +1183,10 @@
         <v>43478.875</v>
       </c>
       <c r="D47">
-        <v>24.84739773643107</v>
+        <v>26.39684882913575</v>
       </c>
       <c r="E47">
-        <v>79.21442905593163</v>
+        <v>80.46140610576489</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1200,10 +1200,10 @@
         <v>43478.91666666666</v>
       </c>
       <c r="D48">
-        <v>24.80108632698058</v>
+        <v>26.44564243425853</v>
       </c>
       <c r="E48">
-        <v>79.22477110119529</v>
+        <v>80.37415427931514</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1217,10 +1217,10 @@
         <v>43478.95833333334</v>
       </c>
       <c r="D49">
-        <v>25.01563365770324</v>
+        <v>26.47540112232232</v>
       </c>
       <c r="E49">
-        <v>79.17324038953207</v>
+        <v>80.33974653389448</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1234,10 +1234,10 @@
         <v>43478</v>
       </c>
       <c r="D50">
-        <v>26.21880899496993</v>
+        <v>26.29934508521576</v>
       </c>
       <c r="E50">
-        <v>78.00919395992415</v>
+        <v>80.12782593549117</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1251,10 +1251,10 @@
         <v>43478.04166666666</v>
       </c>
       <c r="D51">
-        <v>26.50971373501288</v>
+        <v>26.34602092253648</v>
       </c>
       <c r="E51">
-        <v>78.05334439884889</v>
+        <v>80.1318109580974</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1268,10 +1268,10 @@
         <v>43478.08333333334</v>
       </c>
       <c r="D52">
-        <v>26.29941030373624</v>
+        <v>26.28150480507314</v>
       </c>
       <c r="E52">
-        <v>78.07487593630839</v>
+        <v>80.09068650030346</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1285,10 +1285,10 @@
         <v>43478.125</v>
       </c>
       <c r="D53">
-        <v>25.83285328443581</v>
+        <v>26.18689462673374</v>
       </c>
       <c r="E53">
-        <v>78.1283506615838</v>
+        <v>80.16743640935172</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1302,10 +1302,10 @@
         <v>43478.16666666666</v>
       </c>
       <c r="D54">
-        <v>26.34752015448467</v>
+        <v>26.20867329165832</v>
       </c>
       <c r="E54">
-        <v>78.1680547254518</v>
+        <v>80.08702953198943</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1319,10 +1319,10 @@
         <v>43478.20833333334</v>
       </c>
       <c r="D55">
-        <v>26.55553092634059</v>
+        <v>26.22095101462047</v>
       </c>
       <c r="E55">
-        <v>78.00208126772452</v>
+        <v>80.14985254562647</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1336,10 +1336,10 @@
         <v>43478.25</v>
       </c>
       <c r="D56">
-        <v>26.30751034951856</v>
+        <v>26.20976008680698</v>
       </c>
       <c r="E56">
-        <v>78.0294365701921</v>
+        <v>80.01972994198404</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1353,10 +1353,10 @@
         <v>43478.29166666666</v>
       </c>
       <c r="D57">
-        <v>26.57567973333772</v>
+        <v>26.3106355109322</v>
       </c>
       <c r="E57">
-        <v>78.00027283770906</v>
+        <v>79.95116823698774</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1370,10 +1370,10 @@
         <v>43478.33333333334</v>
       </c>
       <c r="D58">
-        <v>26.61107760736508</v>
+        <v>26.33509063901466</v>
       </c>
       <c r="E58">
-        <v>78.2551396165268</v>
+        <v>79.7803087022351</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1387,10 +1387,10 @@
         <v>43478.375</v>
       </c>
       <c r="D59">
-        <v>26.60522247792688</v>
+        <v>26.26823115558502</v>
       </c>
       <c r="E59">
-        <v>78.22415775464485</v>
+        <v>79.93913715615678</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1404,10 +1404,10 @@
         <v>43478.41666666666</v>
       </c>
       <c r="D60">
-        <v>26.63261693865164</v>
+        <v>26.27187283627017</v>
       </c>
       <c r="E60">
-        <v>78.28875896856323</v>
+        <v>79.82604235625381</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1421,10 +1421,10 @@
         <v>43478.45833333334</v>
       </c>
       <c r="D61">
-        <v>26.52983282417602</v>
+        <v>26.44044251460651</v>
       </c>
       <c r="E61">
-        <v>78.35791189214727</v>
+        <v>79.80277585528042</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1438,10 +1438,10 @@
         <v>43478.5</v>
       </c>
       <c r="D62">
-        <v>26.80982215929976</v>
+        <v>26.49364334148436</v>
       </c>
       <c r="E62">
-        <v>78.38200994886141</v>
+        <v>79.7642514689433</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1455,10 +1455,10 @@
         <v>43478.54166666666</v>
       </c>
       <c r="D63">
-        <v>26.79736832535519</v>
+        <v>26.38265537443182</v>
       </c>
       <c r="E63">
-        <v>78.24493219114692</v>
+        <v>79.74996388539191</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1472,10 +1472,10 @@
         <v>43478.58333333334</v>
       </c>
       <c r="D64">
-        <v>26.54635589274351</v>
+        <v>26.170116468708</v>
       </c>
       <c r="E64">
-        <v>78.30861767895718</v>
+        <v>79.67184151516204</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1489,10 +1489,10 @@
         <v>43478.625</v>
       </c>
       <c r="D65">
-        <v>26.68148791356317</v>
+        <v>26.19681605963644</v>
       </c>
       <c r="E65">
-        <v>78.34949497593219</v>
+        <v>79.71198279457474</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1506,10 +1506,10 @@
         <v>43478.66666666666</v>
       </c>
       <c r="D66">
-        <v>26.6146296635837</v>
+        <v>26.26593717552351</v>
       </c>
       <c r="E66">
-        <v>78.26321050207454</v>
+        <v>79.69660705099449</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1523,10 +1523,10 @@
         <v>43478.70833333334</v>
       </c>
       <c r="D67">
-        <v>26.80794552026806</v>
+        <v>26.27312653494717</v>
       </c>
       <c r="E67">
-        <v>78.29882134042678</v>
+        <v>79.75201833556407</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1540,10 +1540,10 @@
         <v>43478.75</v>
       </c>
       <c r="D68">
-        <v>26.54914317456236</v>
+        <v>26.25524445388393</v>
       </c>
       <c r="E68">
-        <v>78.24404799431727</v>
+        <v>79.73936780558292</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1557,10 +1557,10 @@
         <v>43478.79166666666</v>
       </c>
       <c r="D69">
-        <v>26.7958952966522</v>
+        <v>26.24948941451866</v>
       </c>
       <c r="E69">
-        <v>78.31657855716601</v>
+        <v>79.690609030171</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1574,10 +1574,10 @@
         <v>43478.83333333334</v>
       </c>
       <c r="D70">
-        <v>26.73175174490339</v>
+        <v>26.18132302911707</v>
       </c>
       <c r="E70">
-        <v>78.22930697552712</v>
+        <v>79.69835828797582</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1591,10 +1591,10 @@
         <v>43478.875</v>
       </c>
       <c r="D71">
-        <v>26.84064642992756</v>
+        <v>26.24647271389758</v>
       </c>
       <c r="E71">
-        <v>78.37344788248234</v>
+        <v>79.71489071009454</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1608,10 +1608,10 @@
         <v>43478.91666666666</v>
       </c>
       <c r="D72">
-        <v>26.89981665663484</v>
+        <v>26.30176402212908</v>
       </c>
       <c r="E72">
-        <v>78.02445492004264</v>
+        <v>79.76115695834145</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1625,10 +1625,10 @@
         <v>43478.95833333334</v>
       </c>
       <c r="D73">
-        <v>26.54150031006571</v>
+        <v>26.50296905457147</v>
       </c>
       <c r="E73">
-        <v>78.05871502210947</v>
+        <v>79.7188672715818</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1642,10 +1642,10 @@
         <v>43478</v>
       </c>
       <c r="D74">
-        <v>26.7638887032237</v>
+        <v>26.48211246766071</v>
       </c>
       <c r="E74">
-        <v>78.29706573213282</v>
+        <v>79.65468345431772</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1659,10 +1659,10 @@
         <v>43478.04166666666</v>
       </c>
       <c r="D75">
-        <v>26.61563920384025</v>
+        <v>26.44490258890973</v>
       </c>
       <c r="E75">
-        <v>78.48232052908003</v>
+        <v>79.60807874448429</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1676,10 +1676,10 @@
         <v>43478.08333333334</v>
       </c>
       <c r="D76">
-        <v>26.76953938016318</v>
+        <v>26.45828001447062</v>
       </c>
       <c r="E76">
-        <v>78.26058864002277</v>
+        <v>79.56592317837116</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1693,10 +1693,10 @@
         <v>43478.125</v>
       </c>
       <c r="D77">
-        <v>26.63291294852173</v>
+        <v>26.50010350054207</v>
       </c>
       <c r="E77">
-        <v>78.47265837077032</v>
+        <v>79.49307834824538</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1710,10 +1710,10 @@
         <v>43478.16666666666</v>
       </c>
       <c r="D78">
-        <v>26.48012750414385</v>
+        <v>26.27406508360397</v>
       </c>
       <c r="E78">
-        <v>78.23513533634684</v>
+        <v>79.49723584329575</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1727,10 +1727,10 @@
         <v>43478.20833333334</v>
       </c>
       <c r="D79">
-        <v>26.73737953427833</v>
+        <v>26.30190315578721</v>
       </c>
       <c r="E79">
-        <v>78.59574163166472</v>
+        <v>79.65243909041972</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1744,10 +1744,10 @@
         <v>43478.25</v>
       </c>
       <c r="D80">
-        <v>26.82035068021242</v>
+        <v>26.19181757780094</v>
       </c>
       <c r="E80">
-        <v>78.47101093016083</v>
+        <v>79.68947640595141</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1761,10 +1761,10 @@
         <v>43478.29166666666</v>
       </c>
       <c r="D81">
-        <v>26.80741974301855</v>
+        <v>26.09696134206191</v>
       </c>
       <c r="E81">
-        <v>78.54315853268311</v>
+        <v>79.74137112605676</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1778,10 +1778,10 @@
         <v>43478.33333333334</v>
       </c>
       <c r="D82">
-        <v>26.71700626103476</v>
+        <v>26.35497651870596</v>
       </c>
       <c r="E82">
-        <v>78.42955089474604</v>
+        <v>79.76320029699156</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -1795,10 +1795,10 @@
         <v>43478.375</v>
       </c>
       <c r="D83">
-        <v>26.57647856895448</v>
+        <v>26.03244543001319</v>
       </c>
       <c r="E83">
-        <v>78.54749512463849</v>
+        <v>79.72695884694734</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1812,10 +1812,10 @@
         <v>43478.41666666666</v>
       </c>
       <c r="D84">
-        <v>26.54923258973792</v>
+        <v>26.25613638306656</v>
       </c>
       <c r="E84">
-        <v>78.48073056879961</v>
+        <v>79.67487373156256</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1829,10 +1829,10 @@
         <v>43478.45833333334</v>
       </c>
       <c r="D85">
-        <v>26.65245343722389</v>
+        <v>26.25940895900597</v>
       </c>
       <c r="E85">
-        <v>78.50562337240781</v>
+        <v>79.58795452927718</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -1846,10 +1846,10 @@
         <v>43478.5</v>
       </c>
       <c r="D86">
-        <v>26.50434779019538</v>
+        <v>26.26403586515895</v>
       </c>
       <c r="E86">
-        <v>78.55700570711934</v>
+        <v>79.74997230639792</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -1863,10 +1863,10 @@
         <v>43478.54166666666</v>
       </c>
       <c r="D87">
-        <v>26.83919648643461</v>
+        <v>26.10828971002859</v>
       </c>
       <c r="E87">
-        <v>78.43740106661895</v>
+        <v>79.71395075961725</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1880,10 +1880,10 @@
         <v>43478.58333333334</v>
       </c>
       <c r="D88">
-        <v>26.67040374068777</v>
+        <v>26.07440318401992</v>
       </c>
       <c r="E88">
-        <v>78.60220348349942</v>
+        <v>79.60795638383331</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1897,10 +1897,10 @@
         <v>43478.625</v>
       </c>
       <c r="D89">
-        <v>26.67715181595371</v>
+        <v>26.15553694373513</v>
       </c>
       <c r="E89">
-        <v>78.57095173437091</v>
+        <v>79.55707746239749</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1914,10 +1914,10 @@
         <v>43478.66666666666</v>
       </c>
       <c r="D90">
-        <v>26.69558931014213</v>
+        <v>26.02169125186387</v>
       </c>
       <c r="E90">
-        <v>78.48226962788524</v>
+        <v>79.48786407426864</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -1931,10 +1931,10 @@
         <v>43478.70833333334</v>
       </c>
       <c r="D91">
-        <v>26.5555257680852</v>
+        <v>26.01620894273154</v>
       </c>
       <c r="E91">
-        <v>78.43011566185805</v>
+        <v>79.52911223159269</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -1948,10 +1948,10 @@
         <v>43478.75</v>
       </c>
       <c r="D92">
-        <v>26.49290527853533</v>
+        <v>26.12127300068042</v>
       </c>
       <c r="E92">
-        <v>78.59493569184437</v>
+        <v>79.56124441940702</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -1965,10 +1965,10 @@
         <v>43478.79166666666</v>
       </c>
       <c r="D93">
-        <v>26.74957405230888</v>
+        <v>26.15547541360913</v>
       </c>
       <c r="E93">
-        <v>78.49716623708017</v>
+        <v>79.50553917803741</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -1982,10 +1982,10 @@
         <v>43478.83333333334</v>
       </c>
       <c r="D94">
-        <v>26.49727533559046</v>
+        <v>25.97435615241592</v>
       </c>
       <c r="E94">
-        <v>78.58689645215659</v>
+        <v>79.5072515960542</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -1999,10 +1999,10 @@
         <v>43478.875</v>
       </c>
       <c r="D95">
-        <v>26.42238730207647</v>
+        <v>26.06314647671066</v>
       </c>
       <c r="E95">
-        <v>78.563735661923</v>
+        <v>79.47476945877257</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2016,10 +2016,10 @@
         <v>43478.91666666666</v>
       </c>
       <c r="D96">
-        <v>26.42061988261538</v>
+        <v>26.08020346450053</v>
       </c>
       <c r="E96">
-        <v>78.35562500198678</v>
+        <v>79.48596419333063</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2033,10 +2033,10 @@
         <v>43478.95833333334</v>
       </c>
       <c r="D97">
-        <v>26.68734865661385</v>
+        <v>26.35477574698154</v>
       </c>
       <c r="E97">
-        <v>78.25807566185118</v>
+        <v>79.49684472992359</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2050,10 +2050,10 @@
         <v>43478</v>
       </c>
       <c r="D98">
-        <v>24.91348962147636</v>
+        <v>26.7496580314445</v>
       </c>
       <c r="E98">
-        <v>79.49737725576983</v>
+        <v>79.62623146108086</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2067,10 +2067,10 @@
         <v>43478.04166666666</v>
       </c>
       <c r="D99">
-        <v>24.49500753160525</v>
+        <v>26.86192599756631</v>
       </c>
       <c r="E99">
-        <v>79.47585451905024</v>
+        <v>79.61479348921648</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2084,10 +2084,10 @@
         <v>43478.08333333334</v>
       </c>
       <c r="D100">
-        <v>24.48351341597512</v>
+        <v>26.90010154038066</v>
       </c>
       <c r="E100">
-        <v>79.45451932852332</v>
+        <v>79.62297294993861</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2101,10 +2101,10 @@
         <v>43478.125</v>
       </c>
       <c r="D101">
-        <v>24.90250126986017</v>
+        <v>26.78473401405028</v>
       </c>
       <c r="E101">
-        <v>79.31027915560648</v>
+        <v>79.64816742099232</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2118,10 +2118,10 @@
         <v>43478.16666666666</v>
       </c>
       <c r="D102">
-        <v>24.62992248872733</v>
+        <v>26.79769170889726</v>
       </c>
       <c r="E102">
-        <v>79.41324564093686</v>
+        <v>79.58663984789197</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2135,10 +2135,10 @@
         <v>43478.20833333334</v>
       </c>
       <c r="D103">
-        <v>24.98913621184122</v>
+        <v>26.91689198848443</v>
       </c>
       <c r="E103">
-        <v>79.50455014634403</v>
+        <v>79.63617512864369</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2152,10 +2152,10 @@
         <v>43478.25</v>
       </c>
       <c r="D104">
-        <v>24.39185398333323</v>
+        <v>26.85146267568209</v>
       </c>
       <c r="E104">
-        <v>79.4307421137058</v>
+        <v>79.62471478568897</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2169,10 +2169,10 @@
         <v>43478.29166666666</v>
       </c>
       <c r="D105">
-        <v>25.00395512489377</v>
+        <v>26.85480360293121</v>
       </c>
       <c r="E105">
-        <v>79.43843910500433</v>
+        <v>79.62412195103447</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2186,10 +2186,10 @@
         <v>43478.33333333334</v>
       </c>
       <c r="D106">
-        <v>24.47755874653492</v>
+        <v>26.75439172127144</v>
       </c>
       <c r="E106">
-        <v>79.40820729598312</v>
+        <v>79.59320503640298</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2203,10 +2203,10 @@
         <v>43478.375</v>
       </c>
       <c r="D107">
-        <v>24.81863034072396</v>
+        <v>26.859937258109</v>
       </c>
       <c r="E107">
-        <v>79.37866376763984</v>
+        <v>79.62370321364411</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2220,10 +2220,10 @@
         <v>43478.41666666666</v>
       </c>
       <c r="D108">
-        <v>24.75456195904685</v>
+        <v>26.75939005755415</v>
       </c>
       <c r="E108">
-        <v>79.69668124677703</v>
+        <v>79.65202698462748</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2237,10 +2237,10 @@
         <v>43478.45833333334</v>
       </c>
       <c r="D109">
-        <v>24.94306474850163</v>
+        <v>26.77553716614389</v>
       </c>
       <c r="E109">
-        <v>79.34924676645441</v>
+        <v>79.51117371925987</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2254,10 +2254,10 @@
         <v>43478.5</v>
       </c>
       <c r="D110">
-        <v>24.52290609856237</v>
+        <v>26.91559866537403</v>
       </c>
       <c r="E110">
-        <v>79.47466272813233</v>
+        <v>79.64682789651937</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2271,10 +2271,10 @@
         <v>43478.54166666666</v>
       </c>
       <c r="D111">
-        <v>24.91602875335617</v>
+        <v>26.87401156411157</v>
       </c>
       <c r="E111">
-        <v>79.37959815269679</v>
+        <v>79.61897356419587</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2288,10 +2288,10 @@
         <v>43478.58333333334</v>
       </c>
       <c r="D112">
-        <v>24.66173938281301</v>
+        <v>26.83112067409228</v>
       </c>
       <c r="E112">
-        <v>79.42827625424403</v>
+        <v>79.62255164833419</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2305,10 +2305,10 @@
         <v>43478.625</v>
       </c>
       <c r="D113">
-        <v>24.84649755255565</v>
+        <v>26.6933931833954</v>
       </c>
       <c r="E113">
-        <v>79.35710054848398</v>
+        <v>79.6616468421265</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2322,10 +2322,10 @@
         <v>43478.66666666666</v>
       </c>
       <c r="D114">
-        <v>24.65589720071332</v>
+        <v>26.63300181733609</v>
       </c>
       <c r="E114">
-        <v>79.32944089395333</v>
+        <v>79.63052815326819</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2339,10 +2339,10 @@
         <v>43478.70833333334</v>
       </c>
       <c r="D115">
-        <v>24.7055022958217</v>
+        <v>26.60423144393439</v>
       </c>
       <c r="E115">
-        <v>79.37738819995359</v>
+        <v>79.62112916572924</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2356,10 +2356,10 @@
         <v>43478.75</v>
       </c>
       <c r="D116">
-        <v>24.41317563182052</v>
+        <v>26.66437641141266</v>
       </c>
       <c r="E116">
-        <v>79.4591538431294</v>
+        <v>79.56477150219426</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -2373,10 +2373,10 @@
         <v>43478.79166666666</v>
       </c>
       <c r="D117">
-        <v>24.86300565345431</v>
+        <v>26.40905466729091</v>
       </c>
       <c r="E117">
-        <v>79.46884706590535</v>
+        <v>79.61088327080832</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -2390,10 +2390,10 @@
         <v>43478.83333333334</v>
       </c>
       <c r="D118">
-        <v>24.65960866083448</v>
+        <v>26.46221682358017</v>
       </c>
       <c r="E118">
-        <v>79.44489603924097</v>
+        <v>79.51171351610409</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2407,10 +2407,10 @@
         <v>43478.875</v>
       </c>
       <c r="D119">
-        <v>24.90173065772255</v>
+        <v>26.69159353210231</v>
       </c>
       <c r="E119">
-        <v>79.48661412631594</v>
+        <v>79.48550409394119</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -2424,10 +2424,10 @@
         <v>43478.91666666666</v>
       </c>
       <c r="D120">
-        <v>24.96608296267114</v>
+        <v>26.81446869189605</v>
       </c>
       <c r="E120">
-        <v>79.67410133793234</v>
+        <v>79.48548850691751</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -2441,10 +2441,10 @@
         <v>43478.95833333334</v>
       </c>
       <c r="D121">
-        <v>25.09861795486023</v>
+        <v>26.80832599097104</v>
       </c>
       <c r="E121">
-        <v>79.5287455005456</v>
+        <v>79.58006374390574</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2458,10 +2458,10 @@
         <v>43478</v>
       </c>
       <c r="D122">
-        <v>26.34793249350318</v>
+        <v>26.55985286618422</v>
       </c>
       <c r="E122">
-        <v>79.37015201314203</v>
+        <v>80.1470747989414</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -2475,10 +2475,10 @@
         <v>43478.04166666666</v>
       </c>
       <c r="D123">
-        <v>26.64707826690527</v>
+        <v>26.74649095856218</v>
       </c>
       <c r="E123">
-        <v>79.35154889359274</v>
+        <v>80.10087439281227</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -2492,10 +2492,10 @@
         <v>43478.08333333334</v>
       </c>
       <c r="D124">
-        <v>26.62210284821969</v>
+        <v>26.70220753840061</v>
       </c>
       <c r="E124">
-        <v>79.50643556578443</v>
+        <v>80.13787409758524</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -2509,10 +2509,10 @@
         <v>43478.125</v>
       </c>
       <c r="D125">
-        <v>26.77140051037366</v>
+        <v>26.72179033250161</v>
       </c>
       <c r="E125">
-        <v>79.45628327523252</v>
+        <v>80.15643938617252</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -2526,10 +2526,10 @@
         <v>43478.16666666666</v>
       </c>
       <c r="D126">
-        <v>26.66084399592646</v>
+        <v>26.5558223730813</v>
       </c>
       <c r="E126">
-        <v>79.59801087557783</v>
+        <v>80.11386646689968</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -2543,10 +2543,10 @@
         <v>43478.20833333334</v>
       </c>
       <c r="D127">
-        <v>26.66934184920241</v>
+        <v>26.69956214696969</v>
       </c>
       <c r="E127">
-        <v>79.35318711126071</v>
+        <v>80.14846624501007</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -2560,10 +2560,10 @@
         <v>43478.25</v>
       </c>
       <c r="D128">
-        <v>26.69550505049028</v>
+        <v>26.69259621664179</v>
       </c>
       <c r="E128">
-        <v>79.55733765577392</v>
+        <v>80.0885780611311</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -2577,10 +2577,10 @@
         <v>43478.29166666666</v>
       </c>
       <c r="D129">
-        <v>26.76015120192211</v>
+        <v>26.57111001073196</v>
       </c>
       <c r="E129">
-        <v>79.32304731923824</v>
+        <v>80.16510925832355</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -2594,10 +2594,10 @@
         <v>43478.33333333334</v>
       </c>
       <c r="D130">
-        <v>26.72791221383735</v>
+        <v>26.7109357194298</v>
       </c>
       <c r="E130">
-        <v>79.70066155256546</v>
+        <v>80.08833728226999</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -2611,10 +2611,10 @@
         <v>43478.375</v>
       </c>
       <c r="D131">
-        <v>26.59162508992701</v>
+        <v>26.65158326813692</v>
       </c>
       <c r="E131">
-        <v>79.42055117430732</v>
+        <v>80.17750322360337</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -2628,10 +2628,10 @@
         <v>43478.41666666666</v>
       </c>
       <c r="D132">
-        <v>26.57682328596169</v>
+        <v>26.92974875537443</v>
       </c>
       <c r="E132">
-        <v>79.60110044971351</v>
+        <v>80.14180478342216</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -2645,10 +2645,10 @@
         <v>43478.45833333334</v>
       </c>
       <c r="D133">
-        <v>26.78481079170924</v>
+        <v>26.5884269936594</v>
       </c>
       <c r="E133">
-        <v>79.47226641807609</v>
+        <v>80.17472342420588</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -2662,10 +2662,10 @@
         <v>43478.5</v>
       </c>
       <c r="D134">
-        <v>26.66194524932476</v>
+        <v>26.68790255857608</v>
       </c>
       <c r="E134">
-        <v>79.62543674978032</v>
+        <v>80.06727028294786</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -2679,10 +2679,10 @@
         <v>43478.54166666666</v>
       </c>
       <c r="D135">
-        <v>26.59624691874194</v>
+        <v>26.63142090313241</v>
       </c>
       <c r="E135">
-        <v>79.41726211443206</v>
+        <v>80.16932800589707</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -2696,10 +2696,10 @@
         <v>43478.58333333334</v>
       </c>
       <c r="D136">
-        <v>26.64284805021241</v>
+        <v>26.57093095865942</v>
       </c>
       <c r="E136">
-        <v>79.56536171411908</v>
+        <v>80.0808277618397</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -2713,10 +2713,10 @@
         <v>43478.625</v>
       </c>
       <c r="D137">
-        <v>26.70672747076313</v>
+        <v>26.57054455351918</v>
       </c>
       <c r="E137">
-        <v>79.29886890704884</v>
+        <v>80.16745524324226</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -2730,10 +2730,10 @@
         <v>43478.66666666666</v>
       </c>
       <c r="D138">
-        <v>26.48175830212665</v>
+        <v>26.62962716358419</v>
       </c>
       <c r="E138">
-        <v>79.56102695144932</v>
+        <v>80.13521725965749</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -2747,10 +2747,10 @@
         <v>43478.70833333334</v>
       </c>
       <c r="D139">
-        <v>26.50004128996519</v>
+        <v>26.72627852945268</v>
       </c>
       <c r="E139">
-        <v>79.34736497282189</v>
+        <v>80.13158799908292</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -2764,10 +2764,10 @@
         <v>43478.75</v>
       </c>
       <c r="D140">
-        <v>26.82325649032642</v>
+        <v>26.5690338947051</v>
       </c>
       <c r="E140">
-        <v>79.58701471257437</v>
+        <v>80.09138006710386</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -2781,10 +2781,10 @@
         <v>43478.79166666666</v>
       </c>
       <c r="D141">
-        <v>26.79962808747037</v>
+        <v>26.61976162069313</v>
       </c>
       <c r="E141">
-        <v>79.40811638194897</v>
+        <v>80.15410173016507</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -2798,10 +2798,10 @@
         <v>43478.83333333334</v>
       </c>
       <c r="D142">
-        <v>26.54048786480238</v>
+        <v>26.59669739176152</v>
       </c>
       <c r="E142">
-        <v>79.56270818696447</v>
+        <v>80.18571699180623</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -2815,10 +2815,10 @@
         <v>43478.875</v>
       </c>
       <c r="D143">
-        <v>26.66502707321503</v>
+        <v>26.55475187237819</v>
       </c>
       <c r="E143">
-        <v>79.70171212731896</v>
+        <v>80.13767738999488</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -2832,10 +2832,10 @@
         <v>43478.91666666666</v>
       </c>
       <c r="D144">
-        <v>26.68636060271415</v>
+        <v>26.7024053821844</v>
       </c>
       <c r="E144">
-        <v>79.55413758060479</v>
+        <v>80.07647618779153</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -2849,10 +2849,10 @@
         <v>43478.95833333334</v>
       </c>
       <c r="D145">
-        <v>26.75142194645975</v>
+        <v>26.59655971855575</v>
       </c>
       <c r="E145">
-        <v>79.92699809301662</v>
+        <v>80.15487436755519</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -2866,10 +2866,10 @@
         <v>43478</v>
       </c>
       <c r="D146">
-        <v>27.08325188459408</v>
+        <v>27.52250588574408</v>
       </c>
       <c r="E146">
-        <v>79.46754884194981</v>
+        <v>80.53969912738499</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -2883,10 +2883,10 @@
         <v>43478.04166666666</v>
       </c>
       <c r="D147">
-        <v>27.25411986336238</v>
+        <v>27.17429195178088</v>
       </c>
       <c r="E147">
-        <v>79.41380142402777</v>
+        <v>80.53634172376162</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -2900,10 +2900,10 @@
         <v>43478.08333333334</v>
       </c>
       <c r="D148">
-        <v>27.21147929717665</v>
+        <v>27.22554959229587</v>
       </c>
       <c r="E148">
-        <v>79.13717522452082</v>
+        <v>80.45240720180342</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -2917,10 +2917,10 @@
         <v>43478.125</v>
       </c>
       <c r="D149">
-        <v>26.8405092896297</v>
+        <v>27.39762793811305</v>
       </c>
       <c r="E149">
-        <v>79.28961788754771</v>
+        <v>80.44818982768957</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -2934,10 +2934,10 @@
         <v>43478.16666666666</v>
       </c>
       <c r="D150">
-        <v>27.01177683527355</v>
+        <v>27.17592753668083</v>
       </c>
       <c r="E150">
-        <v>79.26491634596128</v>
+        <v>80.39103287117787</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -2951,10 +2951,10 @@
         <v>43478.20833333334</v>
       </c>
       <c r="D151">
-        <v>26.57220225933708</v>
+        <v>27.42682044500168</v>
       </c>
       <c r="E151">
-        <v>79.13660795147524</v>
+        <v>80.47772252452542</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -2968,10 +2968,10 @@
         <v>43478.25</v>
       </c>
       <c r="D152">
-        <v>26.50857265028847</v>
+        <v>27.24082694079647</v>
       </c>
       <c r="E152">
-        <v>79.01973416254086</v>
+        <v>80.42143129696844</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -2985,10 +2985,10 @@
         <v>43478.29166666666</v>
       </c>
       <c r="D153">
-        <v>26.85778469288368</v>
+        <v>27.38927178585892</v>
       </c>
       <c r="E153">
-        <v>78.93941017785545</v>
+        <v>80.4724065344473</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -3002,10 +3002,10 @@
         <v>43478.33333333334</v>
       </c>
       <c r="D154">
-        <v>27.46082622484355</v>
+        <v>27.32862542724884</v>
       </c>
       <c r="E154">
-        <v>78.97327402268445</v>
+        <v>80.48248987583581</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -3019,10 +3019,10 @@
         <v>43478.375</v>
       </c>
       <c r="D155">
-        <v>27.42770847333066</v>
+        <v>27.47274729422994</v>
       </c>
       <c r="E155">
-        <v>78.71309202311193</v>
+        <v>80.46231287653221</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3036,10 +3036,10 @@
         <v>43478.41666666666</v>
       </c>
       <c r="D156">
-        <v>27.43186496975984</v>
+        <v>27.23735128363787</v>
       </c>
       <c r="E156">
-        <v>78.87723351070225</v>
+        <v>80.40325691454045</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -3053,10 +3053,10 @@
         <v>43478.45833333334</v>
       </c>
       <c r="D157">
-        <v>27.54971260552291</v>
+        <v>27.52736576312746</v>
       </c>
       <c r="E157">
-        <v>78.66073674945426</v>
+        <v>80.4802183444645</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -3070,10 +3070,10 @@
         <v>43478.5</v>
       </c>
       <c r="D158">
-        <v>27.44673458572477</v>
+        <v>27.28482844931214</v>
       </c>
       <c r="E158">
-        <v>78.94391571174982</v>
+        <v>80.40613643784809</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -3087,10 +3087,10 @@
         <v>43478.54166666666</v>
       </c>
       <c r="D159">
-        <v>27.43283226092524</v>
+        <v>27.4978489244409</v>
       </c>
       <c r="E159">
-        <v>78.67844316152893</v>
+        <v>80.39712709788421</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -3104,10 +3104,10 @@
         <v>43478.58333333334</v>
       </c>
       <c r="D160">
-        <v>27.27977306732596</v>
+        <v>27.25050469281877</v>
       </c>
       <c r="E160">
-        <v>79.04268631078571</v>
+        <v>80.40831975738166</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -3121,10 +3121,10 @@
         <v>43478.625</v>
       </c>
       <c r="D161">
-        <v>27.36538800904485</v>
+        <v>27.46628937138683</v>
       </c>
       <c r="E161">
-        <v>78.71248545786577</v>
+        <v>80.43027509887308</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -3138,10 +3138,10 @@
         <v>43478.66666666666</v>
       </c>
       <c r="D162">
-        <v>27.40073393172863</v>
+        <v>27.42467875493321</v>
       </c>
       <c r="E162">
-        <v>79.06000940103782</v>
+        <v>80.4752455851993</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -3155,10 +3155,10 @@
         <v>43478.70833333334</v>
       </c>
       <c r="D163">
-        <v>27.24590438216314</v>
+        <v>27.36108149745633</v>
       </c>
       <c r="E163">
-        <v>78.78612950914682</v>
+        <v>80.44564518036286</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -3172,10 +3172,10 @@
         <v>43478.75</v>
       </c>
       <c r="D164">
-        <v>27.36110261945968</v>
+        <v>27.46542140460991</v>
       </c>
       <c r="E164">
-        <v>78.94616331725042</v>
+        <v>80.48337532019366</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -3189,10 +3189,10 @@
         <v>43478.79166666666</v>
       </c>
       <c r="D165">
-        <v>27.47827246804484</v>
+        <v>27.51136559230314</v>
       </c>
       <c r="E165">
-        <v>78.73322339362595</v>
+        <v>80.41379372566196</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -3206,10 +3206,10 @@
         <v>43478.83333333334</v>
       </c>
       <c r="D166">
-        <v>27.45061431478087</v>
+        <v>27.44133853052643</v>
       </c>
       <c r="E166">
-        <v>78.93437990904917</v>
+        <v>80.45337165765368</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -3223,10 +3223,10 @@
         <v>43478.875</v>
       </c>
       <c r="D167">
-        <v>27.24532232534713</v>
+        <v>27.20865421175306</v>
       </c>
       <c r="E167">
-        <v>78.82146434791608</v>
+        <v>80.44929863475613</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -3240,10 +3240,10 @@
         <v>43478.91666666666</v>
       </c>
       <c r="D168">
-        <v>27.53472588525202</v>
+        <v>27.51226760438186</v>
       </c>
       <c r="E168">
-        <v>78.92525092402134</v>
+        <v>80.44716543275845</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -3257,10 +3257,10 @@
         <v>43478.95833333334</v>
       </c>
       <c r="D169">
-        <v>27.37307463412992</v>
+        <v>27.47799293414925</v>
       </c>
       <c r="E169">
-        <v>78.750636430588</v>
+        <v>80.42344405139011</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -3274,10 +3274,10 @@
         <v>43478</v>
       </c>
       <c r="D170">
-        <v>27.73783417353669</v>
+        <v>26.92021284397202</v>
       </c>
       <c r="E170">
-        <v>79.07033084732659</v>
+        <v>79.49111910955669</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -3291,10 +3291,10 @@
         <v>43478.04166666666</v>
       </c>
       <c r="D171">
-        <v>27.72745449960972</v>
+        <v>26.9313952162844</v>
       </c>
       <c r="E171">
-        <v>78.92012961869315</v>
+        <v>79.52035224539767</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -3308,10 +3308,10 @@
         <v>43478.08333333334</v>
       </c>
       <c r="D172">
-        <v>27.77978082018865</v>
+        <v>26.78126181338867</v>
       </c>
       <c r="E172">
-        <v>78.94805176540955</v>
+        <v>79.49577359149775</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -3325,10 +3325,10 @@
         <v>43478.125</v>
       </c>
       <c r="D173">
-        <v>27.68503599676314</v>
+        <v>26.88140097158001</v>
       </c>
       <c r="E173">
-        <v>78.91409842724293</v>
+        <v>79.54232479183828</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -3342,10 +3342,10 @@
         <v>43478.16666666666</v>
       </c>
       <c r="D174">
-        <v>27.68916329598867</v>
+        <v>26.69966220729059</v>
       </c>
       <c r="E174">
-        <v>78.97199880905153</v>
+        <v>79.53338531145491</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -3359,10 +3359,10 @@
         <v>43478.20833333334</v>
       </c>
       <c r="D175">
-        <v>27.62514305669318</v>
+        <v>26.67364786456567</v>
       </c>
       <c r="E175">
-        <v>78.89164576806405</v>
+        <v>79.59536708841443</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -3376,10 +3376,10 @@
         <v>43478.25</v>
       </c>
       <c r="D176">
-        <v>27.74082880813967</v>
+        <v>26.64461667086298</v>
       </c>
       <c r="E176">
-        <v>79.04344420424738</v>
+        <v>79.7269051590017</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -3393,10 +3393,10 @@
         <v>43478.29166666666</v>
       </c>
       <c r="D177">
-        <v>27.784515003727</v>
+        <v>26.71088128549794</v>
       </c>
       <c r="E177">
-        <v>79.0416172884553</v>
+        <v>79.56970471745097</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -3410,10 +3410,10 @@
         <v>43478.33333333334</v>
       </c>
       <c r="D178">
-        <v>27.63123408542393</v>
+        <v>26.55441497387713</v>
       </c>
       <c r="E178">
-        <v>78.92196616278618</v>
+        <v>79.76559210424493</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -3427,10 +3427,10 @@
         <v>43478.375</v>
       </c>
       <c r="D179">
-        <v>27.86317685239003</v>
+        <v>26.64865156190996</v>
       </c>
       <c r="E179">
-        <v>79.03586170785447</v>
+        <v>79.60849795252919</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -3444,10 +3444,10 @@
         <v>43478.41666666666</v>
       </c>
       <c r="D180">
-        <v>27.78772880628715</v>
+        <v>26.59412405531093</v>
       </c>
       <c r="E180">
-        <v>79.02115187354559</v>
+        <v>79.69973218918322</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -3461,10 +3461,10 @@
         <v>43478.45833333334</v>
       </c>
       <c r="D181">
-        <v>27.69789973745889</v>
+        <v>26.57288234073458</v>
       </c>
       <c r="E181">
-        <v>79.02876544070457</v>
+        <v>79.65786312532764</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -3478,10 +3478,10 @@
         <v>43478.5</v>
       </c>
       <c r="D182">
-        <v>27.76149721976265</v>
+        <v>26.7339454927904</v>
       </c>
       <c r="E182">
-        <v>78.8875340561364</v>
+        <v>79.73236897708334</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -3495,10 +3495,10 @@
         <v>43478.54166666666</v>
       </c>
       <c r="D183">
-        <v>27.91820166932324</v>
+        <v>26.64603511127059</v>
       </c>
       <c r="E183">
-        <v>78.99825762553205</v>
+        <v>79.59197081326215</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -3512,10 +3512,10 @@
         <v>43478.58333333334</v>
       </c>
       <c r="D184">
-        <v>27.86255668703298</v>
+        <v>26.6363063863625</v>
       </c>
       <c r="E184">
-        <v>79.03318663643964</v>
+        <v>79.75364115622594</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -3529,10 +3529,10 @@
         <v>43478.625</v>
       </c>
       <c r="D185">
-        <v>27.63552622299679</v>
+        <v>26.68755951769367</v>
       </c>
       <c r="E185">
-        <v>78.89342678406761</v>
+        <v>79.83203144478398</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -3546,10 +3546,10 @@
         <v>43478.66666666666</v>
       </c>
       <c r="D186">
-        <v>27.83218583941597</v>
+        <v>26.56441603544284</v>
       </c>
       <c r="E186">
-        <v>78.92044419384843</v>
+        <v>79.84337258999831</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -3563,10 +3563,10 @@
         <v>43478.70833333334</v>
       </c>
       <c r="D187">
-        <v>27.59412081078776</v>
+        <v>26.65127274216301</v>
       </c>
       <c r="E187">
-        <v>78.99946979546023</v>
+        <v>79.81242323798729</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -3580,10 +3580,10 @@
         <v>43478.75</v>
       </c>
       <c r="D188">
-        <v>27.74666430510087</v>
+        <v>26.59573513101676</v>
       </c>
       <c r="E188">
-        <v>79.05691054639895</v>
+        <v>79.78261227749374</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -3597,10 +3597,10 @@
         <v>43478.79166666666</v>
       </c>
       <c r="D189">
-        <v>27.69636656112565</v>
+        <v>26.59753887326443</v>
       </c>
       <c r="E189">
-        <v>78.90522852080126</v>
+        <v>79.8451428857375</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -3614,10 +3614,10 @@
         <v>43478.83333333334</v>
       </c>
       <c r="D190">
-        <v>27.65487864657658</v>
+        <v>26.56831009300072</v>
       </c>
       <c r="E190">
-        <v>78.98076377008394</v>
+        <v>79.84507565898571</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -3631,10 +3631,10 @@
         <v>43478.875</v>
       </c>
       <c r="D191">
-        <v>27.65065728533655</v>
+        <v>26.62634760559992</v>
       </c>
       <c r="E191">
-        <v>79.03050442400715</v>
+        <v>79.80629676646085</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -3648,10 +3648,10 @@
         <v>43478.91666666666</v>
       </c>
       <c r="D192">
-        <v>27.72525004853564</v>
+        <v>26.65217439096498</v>
       </c>
       <c r="E192">
-        <v>78.90491109402151</v>
+        <v>79.77385676209569</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -3665,10 +3665,10 @@
         <v>43478.95833333334</v>
       </c>
       <c r="D193">
-        <v>27.6699122202137</v>
+        <v>26.81924111777165</v>
       </c>
       <c r="E193">
-        <v>78.93610937232927</v>
+        <v>79.78029616043797</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -3682,10 +3682,10 @@
         <v>43478</v>
       </c>
       <c r="D194">
-        <v>25.60266121654512</v>
+        <v>27.02509405479538</v>
       </c>
       <c r="E194">
-        <v>78.95025546304969</v>
+        <v>80.63425955952302</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -3699,10 +3699,10 @@
         <v>43478.04166666666</v>
       </c>
       <c r="D195">
-        <v>25.55168287905953</v>
+        <v>26.94507259011814</v>
       </c>
       <c r="E195">
-        <v>79.27891904829056</v>
+        <v>80.73179699124043</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -3716,10 +3716,10 @@
         <v>43478.08333333334</v>
       </c>
       <c r="D196">
-        <v>25.528638860796</v>
+        <v>26.96282452641941</v>
       </c>
       <c r="E196">
-        <v>79.00522893900506</v>
+        <v>80.60902491188966</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -3733,10 +3733,10 @@
         <v>43478.125</v>
       </c>
       <c r="D197">
-        <v>25.66574440752775</v>
+        <v>27.13343531381068</v>
       </c>
       <c r="E197">
-        <v>79.1304100642998</v>
+        <v>80.75387098881831</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -3750,10 +3750,10 @@
         <v>43478.16666666666</v>
       </c>
       <c r="D198">
-        <v>25.66290658605439</v>
+        <v>27.23363745790649</v>
       </c>
       <c r="E198">
-        <v>78.94261522410983</v>
+        <v>80.75993678889236</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -3767,10 +3767,10 @@
         <v>43478.20833333334</v>
       </c>
       <c r="D199">
-        <v>25.44272027408147</v>
+        <v>27.08651253491845</v>
       </c>
       <c r="E199">
-        <v>78.71414828510159</v>
+        <v>80.72772889164605</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -3784,10 +3784,10 @@
         <v>43478.25</v>
       </c>
       <c r="D200">
-        <v>25.26185993456134</v>
+        <v>26.94555246534204</v>
       </c>
       <c r="E200">
-        <v>78.75854812228442</v>
+        <v>80.63213594704332</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -3801,10 +3801,10 @@
         <v>43478.29166666666</v>
       </c>
       <c r="D201">
-        <v>25.27330325774967</v>
+        <v>26.99199003877578</v>
       </c>
       <c r="E201">
-        <v>79.00092480580444</v>
+        <v>80.72384272583938</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -3818,10 +3818,10 @@
         <v>43478.33333333334</v>
       </c>
       <c r="D202">
-        <v>25.58528396530361</v>
+        <v>27.32806346854905</v>
       </c>
       <c r="E202">
-        <v>79.05664631283597</v>
+        <v>80.78705681237606</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -3835,10 +3835,10 @@
         <v>43478.375</v>
       </c>
       <c r="D203">
-        <v>25.59389676011245</v>
+        <v>27.13694002012107</v>
       </c>
       <c r="E203">
-        <v>78.76179630090763</v>
+        <v>80.78555722319857</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -3852,10 +3852,10 @@
         <v>43478.41666666666</v>
       </c>
       <c r="D204">
-        <v>25.26918041004884</v>
+        <v>27.00707569077289</v>
       </c>
       <c r="E204">
-        <v>78.81299445975678</v>
+        <v>80.63369882399547</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -3869,10 +3869,10 @@
         <v>43478.45833333334</v>
       </c>
       <c r="D205">
-        <v>25.05223198237784</v>
+        <v>27.15243108958116</v>
       </c>
       <c r="E205">
-        <v>79.06782576694266</v>
+        <v>80.60603386061072</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -3886,10 +3886,10 @@
         <v>43478.5</v>
       </c>
       <c r="D206">
-        <v>25.59514200016926</v>
+        <v>27.24453593192853</v>
       </c>
       <c r="E206">
-        <v>79.03306007495812</v>
+        <v>80.62789325252233</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -3903,10 +3903,10 @@
         <v>43478.54166666666</v>
       </c>
       <c r="D207">
-        <v>25.52687822121892</v>
+        <v>27.23673424943668</v>
       </c>
       <c r="E207">
-        <v>78.74960725859485</v>
+        <v>80.61265131655652</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -3920,10 +3920,10 @@
         <v>43478.58333333334</v>
       </c>
       <c r="D208">
-        <v>25.64065216486868</v>
+        <v>27.22483886111199</v>
       </c>
       <c r="E208">
-        <v>78.88087662273234</v>
+        <v>80.62920879748056</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -3937,10 +3937,10 @@
         <v>43478.625</v>
       </c>
       <c r="D209">
-        <v>25.4478587263715</v>
+        <v>27.32742293004025</v>
       </c>
       <c r="E209">
-        <v>78.7413419115377</v>
+        <v>80.64748024412724</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -3954,10 +3954,10 @@
         <v>43478.66666666666</v>
       </c>
       <c r="D210">
-        <v>25.68882669238078</v>
+        <v>27.20085638429737</v>
       </c>
       <c r="E210">
-        <v>78.96725484971158</v>
+        <v>80.60850153659051</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -3971,10 +3971,10 @@
         <v>43478.70833333334</v>
       </c>
       <c r="D211">
-        <v>25.59744486821674</v>
+        <v>27.34539683749206</v>
       </c>
       <c r="E211">
-        <v>78.77529389863302</v>
+        <v>80.641005571964</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -3988,10 +3988,10 @@
         <v>43478.75</v>
       </c>
       <c r="D212">
-        <v>25.68170887047165</v>
+        <v>27.27959411739131</v>
       </c>
       <c r="E212">
-        <v>78.86362620658345</v>
+        <v>80.61662007359621</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -4005,10 +4005,10 @@
         <v>43478.79166666666</v>
       </c>
       <c r="D213">
-        <v>25.55144519344345</v>
+        <v>27.10292176630072</v>
       </c>
       <c r="E213">
-        <v>78.70583610716425</v>
+        <v>80.6708385484757</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -4022,10 +4022,10 @@
         <v>43478.83333333334</v>
       </c>
       <c r="D214">
-        <v>25.74620379543518</v>
+        <v>26.9566996608588</v>
       </c>
       <c r="E214">
-        <v>78.8644281393542</v>
+        <v>80.78962423054259</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -4039,10 +4039,10 @@
         <v>43478.875</v>
       </c>
       <c r="D215">
-        <v>25.45252016087192</v>
+        <v>27.22470102739583</v>
       </c>
       <c r="E215">
-        <v>78.83275583599773</v>
+        <v>80.79443231213239</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -4056,10 +4056,10 @@
         <v>43478.91666666666</v>
       </c>
       <c r="D216">
-        <v>25.68227041594349</v>
+        <v>27.20076829011814</v>
       </c>
       <c r="E216">
-        <v>79.02522134196496</v>
+        <v>80.76130021379348</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -4073,10 +4073,10 @@
         <v>43478.95833333334</v>
       </c>
       <c r="D217">
-        <v>25.59046829336608</v>
+        <v>27.239083376376</v>
       </c>
       <c r="E217">
-        <v>78.84634238747333</v>
+        <v>80.7107360461238</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -4090,10 +4090,10 @@
         <v>43477.95833333334</v>
       </c>
       <c r="D218">
-        <v>26.44109279609301</v>
+        <v>26.7682407806952</v>
       </c>
       <c r="E218">
-        <v>80.28968366732705</v>
+        <v>79.75077491349529</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -4107,10 +4107,10 @@
         <v>43478</v>
       </c>
       <c r="D219">
-        <v>26.33870746889807</v>
+        <v>26.892847268731</v>
       </c>
       <c r="E219">
-        <v>80.36826892578591</v>
+        <v>79.75604789221455</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -4124,10 +4124,10 @@
         <v>43478.04166666666</v>
       </c>
       <c r="D220">
-        <v>26.37856285209323</v>
+        <v>26.92205894785567</v>
       </c>
       <c r="E220">
-        <v>80.31940626351366</v>
+        <v>79.66636112702858</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -4141,10 +4141,10 @@
         <v>43478.08333333334</v>
       </c>
       <c r="D221">
-        <v>26.33053996689822</v>
+        <v>26.790404361161</v>
       </c>
       <c r="E221">
-        <v>80.37487460753246</v>
+        <v>79.72533528198133</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -4158,10 +4158,10 @@
         <v>43478.125</v>
       </c>
       <c r="D222">
-        <v>26.14826079885065</v>
+        <v>26.7629753715602</v>
       </c>
       <c r="E222">
-        <v>80.21432160451957</v>
+        <v>79.67608556011339</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -4175,10 +4175,10 @@
         <v>43478.16666666666</v>
       </c>
       <c r="D223">
-        <v>26.31035743269687</v>
+        <v>26.76637703378624</v>
       </c>
       <c r="E223">
-        <v>80.49391586124068</v>
+        <v>79.72712826436091</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -4192,10 +4192,10 @@
         <v>43478.20833333334</v>
       </c>
       <c r="D224">
-        <v>26.43551052615794</v>
+        <v>26.78921752172388</v>
       </c>
       <c r="E224">
-        <v>80.28131337816598</v>
+        <v>79.85501596175439</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -4209,10 +4209,10 @@
         <v>43478.25</v>
       </c>
       <c r="D225">
-        <v>26.27543211667768</v>
+        <v>26.85378250547237</v>
       </c>
       <c r="E225">
-        <v>80.37514082991952</v>
+        <v>79.69414625110595</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -4226,10 +4226,10 @@
         <v>43478.29166666666</v>
       </c>
       <c r="D226">
-        <v>26.15555336751069</v>
+        <v>26.89485002741525</v>
       </c>
       <c r="E226">
-        <v>80.26954043508049</v>
+        <v>79.71300062564137</v>
       </c>
     </row>
     <row r="227" spans="1:5">
@@ -4243,10 +4243,10 @@
         <v>43478.33333333334</v>
       </c>
       <c r="D227">
-        <v>26.19812955070347</v>
+        <v>26.82418356837666</v>
       </c>
       <c r="E227">
-        <v>80.51156277528676</v>
+        <v>79.68037938023794</v>
       </c>
     </row>
     <row r="228" spans="1:5">
@@ -4260,10 +4260,10 @@
         <v>43478.375</v>
       </c>
       <c r="D228">
-        <v>26.13572404670241</v>
+        <v>26.82040110698296</v>
       </c>
       <c r="E228">
-        <v>80.19138252085774</v>
+        <v>79.68859404458696</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -4277,10 +4277,10 @@
         <v>43478.41666666666</v>
       </c>
       <c r="D229">
-        <v>26.14864373330425</v>
+        <v>26.88821208360925</v>
       </c>
       <c r="E229">
-        <v>80.3935616999253</v>
+        <v>79.74446896012161</v>
       </c>
     </row>
     <row r="230" spans="1:5">
@@ -4294,10 +4294,10 @@
         <v>43478.45833333334</v>
       </c>
       <c r="D230">
-        <v>26.55129523454639</v>
+        <v>27.00748433780191</v>
       </c>
       <c r="E230">
-        <v>80.39032115856025</v>
+        <v>79.74109626430041</v>
       </c>
     </row>
     <row r="231" spans="1:5">
@@ -4311,10 +4311,10 @@
         <v>43478.5</v>
       </c>
       <c r="D231">
-        <v>26.2657007639694</v>
+        <v>27.05897781745136</v>
       </c>
       <c r="E231">
-        <v>80.46035218982487</v>
+        <v>79.70764590548065</v>
       </c>
     </row>
     <row r="232" spans="1:5">
@@ -4328,10 +4328,10 @@
         <v>43478.54166666666</v>
       </c>
       <c r="D232">
-        <v>26.33433513607503</v>
+        <v>27.1218978640945</v>
       </c>
       <c r="E232">
-        <v>80.20179096625671</v>
+        <v>79.73175603976679</v>
       </c>
     </row>
     <row r="233" spans="1:5">
@@ -4345,10 +4345,10 @@
         <v>43478.58333333334</v>
       </c>
       <c r="D233">
-        <v>26.00618116913411</v>
+        <v>27.06477357202661</v>
       </c>
       <c r="E233">
-        <v>80.163749097505</v>
+        <v>79.7090256685361</v>
       </c>
     </row>
     <row r="234" spans="1:5">
@@ -4362,10 +4362,10 @@
         <v>43478.625</v>
       </c>
       <c r="D234">
-        <v>25.78972477115469</v>
+        <v>26.99282228846212</v>
       </c>
       <c r="E234">
-        <v>80.39177900584706</v>
+        <v>79.6941802808083</v>
       </c>
     </row>
     <row r="235" spans="1:5">
@@ -4379,10 +4379,10 @@
         <v>43478.66666666666</v>
       </c>
       <c r="D235">
-        <v>25.95684743900914</v>
+        <v>26.98894513295362</v>
       </c>
       <c r="E235">
-        <v>80.52816465225635</v>
+        <v>79.72296697070355</v>
       </c>
     </row>
     <row r="236" spans="1:5">
@@ -4396,10 +4396,10 @@
         <v>43478.70833333334</v>
       </c>
       <c r="D236">
-        <v>25.76123856533054</v>
+        <v>27.11998945599132</v>
       </c>
       <c r="E236">
-        <v>80.54421129808618</v>
+        <v>79.75432464635935</v>
       </c>
     </row>
     <row r="237" spans="1:5">
@@ -4413,10 +4413,10 @@
         <v>43478.75</v>
       </c>
       <c r="D237">
-        <v>26.10618547951311</v>
+        <v>27.00793202460897</v>
       </c>
       <c r="E237">
-        <v>80.45202754271644</v>
+        <v>79.73437307135475</v>
       </c>
     </row>
     <row r="238" spans="1:5">
@@ -4430,10 +4430,10 @@
         <v>43478.79166666666</v>
       </c>
       <c r="D238">
-        <v>25.90804097962905</v>
+        <v>27.04446683793615</v>
       </c>
       <c r="E238">
-        <v>80.50847388141183</v>
+        <v>79.82990292472806</v>
       </c>
     </row>
     <row r="239" spans="1:5">
@@ -4447,10 +4447,10 @@
         <v>43478.83333333334</v>
       </c>
       <c r="D239">
-        <v>25.85140840046695</v>
+        <v>27.02686952326908</v>
       </c>
       <c r="E239">
-        <v>80.56110040009023</v>
+        <v>79.77084371291808</v>
       </c>
     </row>
     <row r="240" spans="1:5">
@@ -4464,10 +4464,10 @@
         <v>43478.875</v>
       </c>
       <c r="D240">
-        <v>26.04430260724762</v>
+        <v>26.97626921806396</v>
       </c>
       <c r="E240">
-        <v>80.38468749511283</v>
+        <v>79.768038732907</v>
       </c>
     </row>
     <row r="241" spans="1:5">
@@ -4481,10 +4481,10 @@
         <v>43478.91666666666</v>
       </c>
       <c r="D241">
-        <v>25.76625575838467</v>
+        <v>27.11473555195863</v>
       </c>
       <c r="E241">
-        <v>80.51496935264819</v>
+        <v>79.79668725665718</v>
       </c>
     </row>
     <row r="242" spans="1:5">
@@ -4498,10 +4498,10 @@
         <v>43478.95833333334</v>
       </c>
       <c r="D242">
-        <v>25.8122886949951</v>
+        <v>27.06675983649295</v>
       </c>
       <c r="E242">
-        <v>80.1972211788146</v>
+        <v>79.80548432833773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>